<commit_message>
checked and error free till this
</commit_message>
<xml_diff>
--- a/src/test/resources/exceldata/pythoncodeexcel.xlsx
+++ b/src/test/resources/exceldata/pythoncodeexcel.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26522"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E11BED7-7863-41B7-85C1-86CAD98FC687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Seema\Eclipse\Gitcode\dsalgo\src\test\resources\exceldata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88AE923-A0B8-4B74-BFEE-EA2ABD231610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -55,7 +58,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,16 +406,16 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -420,7 +423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -428,7 +431,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
checked and bug free till this (#13)
</commit_message>
<xml_diff>
--- a/src/test/resources/exceldata/pythoncodeexcel.xlsx
+++ b/src/test/resources/exceldata/pythoncodeexcel.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26522"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E11BED7-7863-41B7-85C1-86CAD98FC687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Seema\Eclipse\Gitcode\dsalgo\src\test\resources\exceldata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88AE923-A0B8-4B74-BFEE-EA2ABD231610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -55,7 +58,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,16 +406,16 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -420,7 +423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -428,7 +431,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>

</xml_diff>